<commit_message>
include 14mv1 stats in 1+2 gallery
</commit_message>
<xml_diff>
--- a/stat/mv2/mv2_stats_workload_update1.xlsx
+++ b/stat/mv2/mv2_stats_workload_update1.xlsx
@@ -12093,6 +12093,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.78</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4.13</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3.48</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4.52</v>
+      </c>
       <c r="L3" s="4">
         <v>3.29</v>
       </c>
@@ -12190,6 +12211,9 @@
       <c r="I5" s="2">
         <v>3.9</v>
       </c>
+      <c r="K5" s="4">
+        <v>5.64</v>
+      </c>
       <c r="L5" s="2">
         <v>3.75</v>
       </c>
@@ -12287,6 +12311,9 @@
       <c r="I7" s="2">
         <v>3.93</v>
       </c>
+      <c r="K7" s="4">
+        <v>5.1</v>
+      </c>
       <c r="L7" s="2">
         <v>3.97</v>
       </c>
@@ -12384,6 +12411,9 @@
       <c r="I9" s="2">
         <v>4.48</v>
       </c>
+      <c r="K9" s="4">
+        <v>5.65</v>
+      </c>
       <c r="L9" s="2">
         <v>3.85</v>
       </c>
@@ -12481,6 +12511,9 @@
       <c r="I11" s="2">
         <v>3.99</v>
       </c>
+      <c r="K11" s="4">
+        <v>6.47</v>
+      </c>
       <c r="L11" s="2">
         <v>4.63</v>
       </c>
@@ -12578,6 +12611,9 @@
       <c r="I13" s="2">
         <v>4.2</v>
       </c>
+      <c r="K13" s="4">
+        <v>6.92</v>
+      </c>
       <c r="L13" s="2">
         <v>4.47</v>
       </c>
@@ -12675,6 +12711,9 @@
       <c r="I15" s="2">
         <v>4.55</v>
       </c>
+      <c r="K15" s="4">
+        <v>5.66</v>
+      </c>
       <c r="L15" s="2">
         <v>4.26</v>
       </c>
@@ -12771,6 +12810,9 @@
       </c>
       <c r="I17" s="2">
         <v>2.68</v>
+      </c>
+      <c r="K17" s="4">
+        <v>4.45</v>
       </c>
       <c r="L17" s="2">
         <v>3.96</v>
@@ -12862,6 +12904,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>6.71</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.69</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5.66</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6.98</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5.12</v>
+      </c>
+      <c r="H3" s="4">
+        <v>6.25</v>
+      </c>
+      <c r="I3" s="4">
+        <v>8.890000000000001</v>
+      </c>
       <c r="L3" s="4">
         <v>3.93</v>
       </c>
@@ -12959,6 +13022,9 @@
       <c r="I5" s="2">
         <v>6.08</v>
       </c>
+      <c r="K5" s="4">
+        <v>8.69</v>
+      </c>
       <c r="L5" s="2">
         <v>5.04</v>
       </c>
@@ -13056,6 +13122,9 @@
       <c r="I7" s="2">
         <v>6.33</v>
       </c>
+      <c r="K7" s="4">
+        <v>9.07</v>
+      </c>
       <c r="L7" s="2">
         <v>5.21</v>
       </c>
@@ -13153,6 +13222,9 @@
       <c r="I9" s="2">
         <v>7.8</v>
       </c>
+      <c r="K9" s="4">
+        <v>10.21</v>
+      </c>
       <c r="L9" s="2">
         <v>5.24</v>
       </c>
@@ -13250,6 +13322,9 @@
       <c r="I11" s="2">
         <v>6.24</v>
       </c>
+      <c r="K11" s="4">
+        <v>11.32</v>
+      </c>
       <c r="L11" s="2">
         <v>7.41</v>
       </c>
@@ -13347,6 +13422,9 @@
       <c r="I13" s="2">
         <v>6.79</v>
       </c>
+      <c r="K13" s="4">
+        <v>11.04</v>
+      </c>
       <c r="L13" s="2">
         <v>6.05</v>
       </c>
@@ -13444,6 +13522,9 @@
       <c r="I15" s="2">
         <v>7.42</v>
       </c>
+      <c r="K15" s="4">
+        <v>9.16</v>
+      </c>
       <c r="L15" s="2">
         <v>6</v>
       </c>
@@ -13540,6 +13621,9 @@
       </c>
       <c r="I17" s="2">
         <v>3.16</v>
+      </c>
+      <c r="K17" s="4">
+        <v>8.56</v>
       </c>
       <c r="L17" s="2">
         <v>5.53</v>
@@ -13631,6 +13715,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>8.42</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.72</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9.43</v>
+      </c>
+      <c r="G3" s="4">
+        <v>8.58</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7.51</v>
+      </c>
+      <c r="I3" s="4">
+        <v>11.88</v>
+      </c>
       <c r="L3" s="4">
         <v>5.98</v>
       </c>
@@ -13728,6 +13833,9 @@
       <c r="I5" s="2">
         <v>8.69</v>
       </c>
+      <c r="K5" s="4">
+        <v>11.47</v>
+      </c>
       <c r="L5" s="2">
         <v>6.69</v>
       </c>
@@ -13825,6 +13933,9 @@
       <c r="I7" s="2">
         <v>8.1</v>
       </c>
+      <c r="K7" s="4">
+        <v>12.03</v>
+      </c>
       <c r="L7" s="2">
         <v>7.82</v>
       </c>
@@ -13922,6 +14033,9 @@
       <c r="I9" s="2">
         <v>10.7</v>
       </c>
+      <c r="K9" s="4">
+        <v>13.25</v>
+      </c>
       <c r="L9" s="2">
         <v>7.59</v>
       </c>
@@ -14019,6 +14133,9 @@
       <c r="I11" s="2">
         <v>8.380000000000001</v>
       </c>
+      <c r="K11" s="4">
+        <v>13.9</v>
+      </c>
       <c r="L11" s="2">
         <v>9.9</v>
       </c>
@@ -14116,6 +14233,9 @@
       <c r="I13" s="2">
         <v>8.25</v>
       </c>
+      <c r="K13" s="4">
+        <v>14.42</v>
+      </c>
       <c r="L13" s="2">
         <v>8.06</v>
       </c>
@@ -14213,6 +14333,9 @@
       <c r="I15" s="2">
         <v>9.6</v>
       </c>
+      <c r="K15" s="4">
+        <v>12.18</v>
+      </c>
       <c r="L15" s="2">
         <v>7.7</v>
       </c>
@@ -14309,6 +14432,9 @@
       </c>
       <c r="I17" s="2">
         <v>4.92</v>
+      </c>
+      <c r="K17" s="4">
+        <v>11.32</v>
       </c>
       <c r="L17" s="2">
         <v>7.24</v>
@@ -14400,6 +14526,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>10.18</v>
+      </c>
+      <c r="D3" s="4">
+        <v>11.39</v>
+      </c>
+      <c r="E3" s="4">
+        <v>7.32</v>
+      </c>
+      <c r="F3" s="4">
+        <v>11.41</v>
+      </c>
+      <c r="G3" s="4">
+        <v>12.33</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8.609999999999999</v>
+      </c>
+      <c r="I3" s="4">
+        <v>15.96</v>
+      </c>
       <c r="L3" s="4">
         <v>7.84</v>
       </c>
@@ -14497,6 +14644,9 @@
       <c r="I5" s="2">
         <v>14.35</v>
       </c>
+      <c r="K5" s="4">
+        <v>14.09</v>
+      </c>
       <c r="L5" s="2">
         <v>8.99</v>
       </c>
@@ -14594,6 +14744,9 @@
       <c r="I7" s="2">
         <v>15.02</v>
       </c>
+      <c r="K7" s="4">
+        <v>15.04</v>
+      </c>
       <c r="L7" s="2">
         <v>9.69</v>
       </c>
@@ -14691,6 +14844,9 @@
       <c r="I9" s="2">
         <v>16.41</v>
       </c>
+      <c r="K9" s="4">
+        <v>17.95</v>
+      </c>
       <c r="L9" s="2">
         <v>11.22</v>
       </c>
@@ -14788,6 +14944,9 @@
       <c r="I11" s="2">
         <v>16.82</v>
       </c>
+      <c r="K11" s="4">
+        <v>19.04</v>
+      </c>
       <c r="L11" s="2">
         <v>14.14</v>
       </c>
@@ -14885,6 +15044,9 @@
       <c r="I13" s="2">
         <v>15.02</v>
       </c>
+      <c r="K13" s="4">
+        <v>19.52</v>
+      </c>
       <c r="L13" s="2">
         <v>12.91</v>
       </c>
@@ -14982,6 +15144,9 @@
       <c r="I15" s="2">
         <v>15.66</v>
       </c>
+      <c r="K15" s="4">
+        <v>16.78</v>
+      </c>
       <c r="L15" s="2">
         <v>13.77</v>
       </c>
@@ -15078,6 +15243,9 @@
       </c>
       <c r="I17" s="2">
         <v>6.27</v>
+      </c>
+      <c r="K17" s="4">
+        <v>13.5</v>
       </c>
       <c r="L17" s="2">
         <v>10.72</v>
@@ -15169,6 +15337,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>6.67</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.47</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5.172413793103448</v>
+      </c>
+      <c r="F3" s="4">
+        <v>7.35</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10.33</v>
+      </c>
+      <c r="H3" s="4">
+        <v>6.16</v>
+      </c>
+      <c r="I3" s="4">
+        <v>7.92</v>
+      </c>
       <c r="L3" s="4">
         <v>5.46875</v>
       </c>
@@ -15266,6 +15455,9 @@
       <c r="I5" s="2">
         <v>5.705882352941177</v>
       </c>
+      <c r="K5" s="4">
+        <v>7.31</v>
+      </c>
       <c r="L5" s="2">
         <v>5.903225806451613</v>
       </c>
@@ -15363,6 +15555,9 @@
       <c r="I7" s="2">
         <v>9.550000000000001</v>
       </c>
+      <c r="K7" s="4">
+        <v>11.75</v>
+      </c>
       <c r="L7" s="2">
         <v>7.285714285714286</v>
       </c>
@@ -15460,6 +15655,9 @@
       <c r="I9" s="2">
         <v>7.982758620689655</v>
       </c>
+      <c r="K9" s="4">
+        <v>11.39</v>
+      </c>
       <c r="L9" s="2">
         <v>7.46</v>
       </c>
@@ -15557,6 +15755,9 @@
       <c r="I11" s="2">
         <v>10.88</v>
       </c>
+      <c r="K11" s="4">
+        <v>12.18</v>
+      </c>
       <c r="L11" s="2">
         <v>7.845070422535211</v>
       </c>
@@ -15654,6 +15855,9 @@
       <c r="I13" s="2">
         <v>8.77</v>
       </c>
+      <c r="K13" s="4">
+        <v>12.85</v>
+      </c>
       <c r="L13" s="2">
         <v>8.56</v>
       </c>
@@ -15751,6 +15955,9 @@
       <c r="I15" s="2">
         <v>7.235294117647059</v>
       </c>
+      <c r="K15" s="4">
+        <v>12.86</v>
+      </c>
       <c r="L15" s="2">
         <v>9.720000000000001</v>
       </c>
@@ -15847,6 +16054,9 @@
       </c>
       <c r="I17" s="2">
         <v>6.2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>8.82</v>
       </c>
       <c r="L17" s="2">
         <v>8.34</v>
@@ -15938,6 +16148,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>8.66</v>
+      </c>
+      <c r="D3" s="4">
+        <v>10.06</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.340909090909091</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10.07</v>
+      </c>
+      <c r="G3" s="4">
+        <v>12.05</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8.66</v>
+      </c>
+      <c r="I3" s="4">
+        <v>12.53</v>
+      </c>
       <c r="L3" s="4">
         <v>6.254237288135593</v>
       </c>
@@ -16035,6 +16266,9 @@
       <c r="I5" s="2">
         <v>7.914285714285715</v>
       </c>
+      <c r="K5" s="4">
+        <v>11.52</v>
+      </c>
       <c r="L5" s="2">
         <v>7.18</v>
       </c>
@@ -16132,6 +16366,9 @@
       <c r="I7" s="2">
         <v>13.51</v>
       </c>
+      <c r="K7" s="4">
+        <v>14.38</v>
+      </c>
       <c r="L7" s="2">
         <v>8.31764705882353</v>
       </c>
@@ -16229,6 +16466,9 @@
       <c r="I9" s="2">
         <v>11.25555555555556</v>
       </c>
+      <c r="K9" s="4">
+        <v>15.23</v>
+      </c>
       <c r="L9" s="2">
         <v>9.26</v>
       </c>
@@ -16326,6 +16566,9 @@
       <c r="I11" s="2">
         <v>16.04</v>
       </c>
+      <c r="K11" s="4">
+        <v>16.22</v>
+      </c>
       <c r="L11" s="2">
         <v>10.30769230769231</v>
       </c>
@@ -16423,6 +16666,9 @@
       <c r="I13" s="2">
         <v>13.48</v>
       </c>
+      <c r="K13" s="4">
+        <v>16.63</v>
+      </c>
       <c r="L13" s="2">
         <v>9.719101123595506</v>
       </c>
@@ -16520,6 +16766,9 @@
       <c r="I15" s="2">
         <v>10.83333333333333</v>
       </c>
+      <c r="K15" s="4">
+        <v>16.76</v>
+      </c>
       <c r="L15" s="2">
         <v>12.92</v>
       </c>
@@ -16616,6 +16865,9 @@
       </c>
       <c r="I17" s="2">
         <v>6.65</v>
+      </c>
+      <c r="K17" s="4">
+        <v>12.13</v>
       </c>
       <c r="L17" s="2">
         <v>11.57</v>
@@ -17254,6 +17506,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>12.15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.209302325581396</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12.33</v>
+      </c>
+      <c r="G3" s="4">
+        <v>15.34</v>
+      </c>
+      <c r="H3" s="4">
+        <v>9.94</v>
+      </c>
+      <c r="I3" s="4">
+        <v>14.37</v>
+      </c>
       <c r="L3" s="4">
         <v>7.12280701754386</v>
       </c>
@@ -17351,6 +17624,9 @@
       <c r="I5" s="2">
         <v>11.63</v>
       </c>
+      <c r="K5" s="4">
+        <v>13.41</v>
+      </c>
       <c r="L5" s="2">
         <v>8.095238095238095</v>
       </c>
@@ -17448,6 +17724,9 @@
       <c r="I7" s="2">
         <v>16.21</v>
       </c>
+      <c r="K7" s="4">
+        <v>17.42</v>
+      </c>
       <c r="L7" s="2">
         <v>9.359999999999999</v>
       </c>
@@ -17545,6 +17824,9 @@
       <c r="I9" s="2">
         <v>15.24</v>
       </c>
+      <c r="K9" s="4">
+        <v>19.57</v>
+      </c>
       <c r="L9" s="2">
         <v>12.38</v>
       </c>
@@ -17642,6 +17924,9 @@
       <c r="I11" s="2">
         <v>21.53</v>
       </c>
+      <c r="K11" s="4">
+        <v>21.51</v>
+      </c>
       <c r="L11" s="2">
         <v>11.9</v>
       </c>
@@ -17739,6 +18024,9 @@
       <c r="I13" s="2">
         <v>16.32</v>
       </c>
+      <c r="K13" s="4">
+        <v>21.16</v>
+      </c>
       <c r="L13" s="2">
         <v>12.51</v>
       </c>
@@ -17836,6 +18124,9 @@
       <c r="I15" s="2">
         <v>12.27</v>
       </c>
+      <c r="K15" s="4">
+        <v>20.24</v>
+      </c>
       <c r="L15" s="2">
         <v>16.32</v>
       </c>
@@ -17932,6 +18223,9 @@
       </c>
       <c r="I17" s="2">
         <v>7.35</v>
+      </c>
+      <c r="K17" s="4">
+        <v>13.06</v>
       </c>
       <c r="L17" s="2">
         <v>12.32</v>
@@ -18023,6 +18317,27 @@
       </c>
     </row>
     <row r="3" spans="2:18">
+      <c r="C3" s="4">
+        <v>13.36</v>
+      </c>
+      <c r="D3" s="4">
+        <v>16.02</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.69</v>
+      </c>
+      <c r="F3" s="4">
+        <v>17.09</v>
+      </c>
+      <c r="G3" s="4">
+        <v>22.52</v>
+      </c>
+      <c r="H3" s="4">
+        <v>12.56</v>
+      </c>
+      <c r="I3" s="4">
+        <v>19.75</v>
+      </c>
       <c r="L3" s="4">
         <v>8.415584415584416</v>
       </c>
@@ -18120,6 +18435,9 @@
       <c r="I5" s="2">
         <v>16.2</v>
       </c>
+      <c r="K5" s="4">
+        <v>17.38</v>
+      </c>
       <c r="L5" s="2">
         <v>10.65</v>
       </c>
@@ -18217,6 +18535,9 @@
       <c r="I7" s="2">
         <v>22.85</v>
       </c>
+      <c r="K7" s="4">
+        <v>23.41</v>
+      </c>
       <c r="L7" s="2">
         <v>11.84</v>
       </c>
@@ -18314,6 +18635,9 @@
       <c r="I9" s="2">
         <v>21.03</v>
       </c>
+      <c r="K9" s="4">
+        <v>27.46</v>
+      </c>
       <c r="L9" s="2">
         <v>15.94</v>
       </c>
@@ -18411,6 +18735,9 @@
       <c r="I11" s="2">
         <v>26.98</v>
       </c>
+      <c r="K11" s="4">
+        <v>29.29</v>
+      </c>
       <c r="L11" s="2">
         <v>14.45</v>
       </c>
@@ -18508,6 +18835,9 @@
       <c r="I13" s="2">
         <v>21.23</v>
       </c>
+      <c r="K13" s="4">
+        <v>30</v>
+      </c>
       <c r="L13" s="2">
         <v>16.13</v>
       </c>
@@ -18605,6 +18935,9 @@
       <c r="I15" s="2">
         <v>20.67</v>
       </c>
+      <c r="K15" s="4">
+        <v>28.87</v>
+      </c>
       <c r="L15" s="2">
         <v>19.45</v>
       </c>
@@ -18701,6 +19034,9 @@
       </c>
       <c r="I17" s="2">
         <v>9.148148148148149</v>
+      </c>
+      <c r="K17" s="4">
+        <v>21.96</v>
       </c>
       <c r="L17" s="2">
         <v>17.69</v>

</xml_diff>